<commit_message>
arreglo a sp y reporte
se modifica reporte ya que se tuvo que modificar sp ya que tenia un waitfor y eso hacia que los datos tomados de las muestras fuerean erroneos al compararlo al ORM
</commit_message>
<xml_diff>
--- a/nodejsapi/Report.xlsx
+++ b/nodejsapi/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Desktop\Work\2023 S1\BDI\Repositories\BDI_CASO_3_PRELIMINAR_4\nodejsapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10916B9C-4007-498B-BEA9-C07469574DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD55D09-5A4B-48D5-9496-01E4A700F675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B5F31570-9163-483A-A18B-5C878F5082A1}"/>
   </bookViews>
@@ -98,26 +98,26 @@
     <t>Figura 6: Tabla de resultado de Jmeter</t>
   </si>
   <si>
-    <t>Como se puede observar, se realizaron 200 ejecuciones totales para la prueba, el tiempo medio fue de 4021 ms.</t>
-  </si>
-  <si>
-    <t>Como se puede observar, se realizaron 200 ejecuciones totales para la prueba, el tiempo medio fue de 2612 ms.</t>
-  </si>
-  <si>
     <t>Conclusiones:</t>
   </si>
   <si>
     <t>Como se puede observar, se realizaron 200 ejecuciones totales para la prueba, el tiempo medio fue de 424 ms.</t>
   </si>
   <si>
-    <t>La seleccion de un modo de conexion depende de varios aspectos a tomar en cuenta, por ejemplo escalabilidad, concurrencia, velocidad, etc. Como se puede observar el endpoint con mejor tiempo corresponde al ORM seguido del connection sin pooling y finalmente el connection con pooling. ¿Quiere decir que alguna es mejor que la otra? No, esto va a depender como se menciono de los requerimientos del proyecto. Muchas veces es mejor optar por endpoints con pooling ya que se manejan las conexiones de una forma más ordenada y se pueden llegar a reutilizar, por lo que es el preferido para proyectos con una gran escalabilidad y concurrencia. Por otro lado si lo que se desea es una conexion sencilla y rapida, se podria optar por conexiones sin pooling, esto podria darse en un StartUp o en request que se sabe no tienen mucha recurrencia, ya que abrir y mantener un pooling cuesta recursos y debe darse sin tanta concurrencia ya que va a lleagr un punto donde ya no se van a poder abrir más conexiones al mismo tiempo. Finalmente el ORM utilizado utilizaba conexiones con pooling por lo que cuenta con las ventajas de este y además logro el mejor tiempo y fue el de programación más sencilla. Por lo que esta ultima es una buena opción para gente no tan experimentada con el lenguaje SQL.</t>
+    <t>Como se puede observar, se realizaron 200 ejecuciones totales para la prueba, el tiempo medio fue de 372 ms.</t>
+  </si>
+  <si>
+    <t>La selección de un modo de conexión depende de varios aspectos a tomar en cuenta, por ejemplo, escalabilidad, concurrencia, velocidad, etc. Como se puede observar el endpoint con mejor tiempo corresponde endpoint con pooling seguido del endpoint con ORM y finalmente el endpoint sin pooling. ¿Quiere decir que alguna es mejor que la otra? No, esto va a depender como se mencionó de los requerimientos del proyecto. Muchas veces es mejor optar por endpoints con pooling ya que se manejan las conexiones de una forma más ordenada y se pueden llegar a reutilizar, por lo que es el preferido para proyectos con una gran escalabilidad y concurrencia. Por otro lado, si lo que se desea es una conexión sencilla y rápida, se podría optar por conexiones sin pooling, esto podria darse en un StartUp o en request que se sabe no tienen mucha recurrencia, ya que abrir y mantener un pooling a pesar de las ventajas, cuesta recursos. Finalmente, el ORM utiliza conexiones con pooling por lo que cuenta con las ventajas de este y además logro el mejor tiempo y fue el de programación más sencilla. Por lo que esta última es una buena opción para gente no tan experimentada con el lenguaje SQL.</t>
+  </si>
+  <si>
+    <t>Como se puede observar, se realizaron 200 ejecuciones totales para la prueba, el tiempo medio fue de 570 ms.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +128,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,24 +216,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -236,13 +225,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,128 +449,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7326</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>14655</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>146538</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>169942</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0556496-12EE-61F9-7F87-1C3971BBCBF6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3656134" y="4967655"/>
-          <a:ext cx="6220558" cy="536287"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>14653</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>157938</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B1E7B0-60AD-FA3F-38A7-314AF07518A9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10946424" y="5158153"/>
-          <a:ext cx="6081345" cy="524285"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>7327</xdr:colOff>
       <xdr:row>26</xdr:row>
@@ -589,7 +474,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -605,6 +490,111 @@
         <a:xfrm>
           <a:off x="17643231" y="5143499"/>
           <a:ext cx="6572250" cy="558150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>109904</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EF8ED80-A231-FAEC-9359-ABBCA6F4515E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10953750" y="5143502"/>
+          <a:ext cx="6183923" cy="548446"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>168519</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D56E7D49-161C-6E10-E2CF-1759566CE8FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3648808" y="4960327"/>
+          <a:ext cx="6249865" cy="546855"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -926,26 +916,26 @@
   <dimension ref="B2:AT32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AN4" sqref="AN4"/>
+      <selection activeCell="AN26" sqref="AN26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="2" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
       <c r="S2" s="4" t="s">
         <v>9</v>
       </c>
@@ -954,55 +944,55 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
-      <c r="AD2" s="10" t="s">
+      <c r="AD2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AO2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP2" s="8"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AO2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP2" s="2"/>
     </row>
     <row r="3" spans="2:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="G3" s="5" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="S3" s="6" t="s">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="S3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="AD3" s="11" t="s">
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="AD3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="11"/>
-      <c r="AJ3" s="11"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
       <c r="AO3" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AP3" s="12"/>
       <c r="AQ3" s="12"/>
@@ -1011,33 +1001,33 @@
       <c r="AT3" s="12"/>
     </row>
     <row r="4" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
       <c r="AO4" s="12"/>
       <c r="AP4" s="12"/>
       <c r="AQ4" s="12"/>
@@ -1046,33 +1036,33 @@
       <c r="AT4" s="12"/>
     </row>
     <row r="5" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
       <c r="AO5" s="12"/>
       <c r="AP5" s="12"/>
       <c r="AQ5" s="12"/>
@@ -1081,26 +1071,26 @@
       <c r="AT5" s="12"/>
     </row>
     <row r="6" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
-      <c r="AJ6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
       <c r="AO6" s="12"/>
       <c r="AP6" s="12"/>
       <c r="AQ6" s="12"/>
@@ -1109,14 +1099,14 @@
       <c r="AT6" s="12"/>
     </row>
     <row r="7" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
       <c r="AO7" s="12"/>
       <c r="AP7" s="12"/>
       <c r="AQ7" s="12"/>
@@ -1133,14 +1123,14 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
-      <c r="AD8" s="10" t="s">
+      <c r="AD8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AE8" s="10"/>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="10"/>
-      <c r="AI8" s="10"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
       <c r="AO8" s="12"/>
       <c r="AP8" s="12"/>
       <c r="AQ8" s="12"/>
@@ -1229,16 +1219,16 @@
       <c r="AT18" s="12"/>
     </row>
     <row r="19" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="S19" s="9" t="s">
+      <c r="S19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
       <c r="AO19" s="12"/>
       <c r="AP19" s="12"/>
       <c r="AQ19" s="12"/>
@@ -1247,34 +1237,34 @@
       <c r="AT19" s="12"/>
     </row>
     <row r="20" spans="7:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AD20" s="7" t="s">
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AD20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AE20" s="7"/>
-      <c r="AF20" s="7"/>
-      <c r="AG20" s="7"/>
-      <c r="AH20" s="7"/>
-      <c r="AI20" s="7"/>
-      <c r="AJ20" s="7"/>
-      <c r="AK20" s="7"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
       <c r="AO20" s="12"/>
       <c r="AP20" s="12"/>
       <c r="AQ20" s="12"/>
@@ -1283,30 +1273,30 @@
       <c r="AT20" s="12"/>
     </row>
     <row r="21" spans="7:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
-      <c r="AI21" s="7"/>
-      <c r="AJ21" s="7"/>
-      <c r="AK21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
       <c r="AO21" s="12"/>
       <c r="AP21" s="12"/>
       <c r="AQ21" s="12"/>
@@ -1315,30 +1305,30 @@
       <c r="AT21" s="12"/>
     </row>
     <row r="22" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
-      <c r="AF22" s="7"/>
-      <c r="AG22" s="7"/>
-      <c r="AH22" s="7"/>
-      <c r="AI22" s="7"/>
-      <c r="AJ22" s="7"/>
-      <c r="AK22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
       <c r="AO22" s="12"/>
       <c r="AP22" s="12"/>
       <c r="AQ22" s="12"/>
@@ -1347,30 +1337,30 @@
       <c r="AT22" s="12"/>
     </row>
     <row r="23" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-      <c r="AH23" s="7"/>
-      <c r="AI23" s="7"/>
-      <c r="AJ23" s="7"/>
-      <c r="AK23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
       <c r="AO23" s="12"/>
       <c r="AP23" s="12"/>
       <c r="AQ23" s="12"/>
@@ -1379,30 +1369,30 @@
       <c r="AT23" s="12"/>
     </row>
     <row r="24" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
-      <c r="AJ24" s="7"/>
-      <c r="AK24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
       <c r="AO24" s="12"/>
       <c r="AP24" s="12"/>
       <c r="AQ24" s="12"/>
@@ -1411,32 +1401,32 @@
       <c r="AT24" s="12"/>
     </row>
     <row r="25" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AD25" s="7"/>
-      <c r="AE25" s="7"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="7"/>
-      <c r="AH25" s="7"/>
-      <c r="AI25" s="7"/>
-      <c r="AJ25" s="7"/>
-      <c r="AK25" s="7"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
     </row>
     <row r="26" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
     </row>
     <row r="27" spans="7:46" x14ac:dyDescent="0.25">
       <c r="S27" s="4" t="s">
@@ -1447,77 +1437,91 @@
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
-      <c r="AD27" s="10" t="s">
+      <c r="AD27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AE27" s="10"/>
-      <c r="AF27" s="10"/>
-      <c r="AG27" s="10"/>
-      <c r="AH27" s="10"/>
-      <c r="AI27" s="10"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
     </row>
     <row r="30" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="7:46" x14ac:dyDescent="0.25">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="S31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AD31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="S31" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AD31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
-      <c r="AJ31" s="7"/>
-      <c r="AK31" s="7"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
     </row>
     <row r="32" spans="7:46" x14ac:dyDescent="0.25">
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="7"/>
-      <c r="AH32" s="7"/>
-      <c r="AI32" s="7"/>
-      <c r="AJ32" s="7"/>
-      <c r="AK32" s="7"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+      <c r="AK32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="G30:N31"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="G3:M5"/>
+    <mergeCell ref="S3:Y6"/>
+    <mergeCell ref="S8:X8"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="G20:N24"/>
     <mergeCell ref="AD31:AK32"/>
     <mergeCell ref="AO2:AP2"/>
     <mergeCell ref="S19:Z25"/>
@@ -1529,22 +1533,9 @@
     <mergeCell ref="AD20:AK25"/>
     <mergeCell ref="AD27:AI27"/>
     <mergeCell ref="AO3:AT24"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="G30:N31"/>
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="G3:M5"/>
-    <mergeCell ref="S3:Y6"/>
-    <mergeCell ref="S8:X8"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="G20:N24"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>